<commit_message>
Corrected FREESTATE in num_lines
</commit_message>
<xml_diff>
--- a/data/num_lines.xlsx
+++ b/data/num_lines.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\pypsa-za\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DAF7DC71-3E1C-486F-ADAE-7723C96E8EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3029A53-E9CC-429D-8198-1F5404DC4800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21340"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RSA" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="42">
   <si>
     <t>name</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>NORTH WEST</t>
-  </si>
-  <si>
-    <t>FREESTATE</t>
   </si>
   <si>
     <t>GAUTENG</t>
@@ -156,7 +153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -990,10 +987,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -1025,11 +1022,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1163,7 +1160,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -1186,7 +1183,7 @@
         <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1206,7 +1203,7 @@
         <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -1223,10 +1220,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
         <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1243,10 +1240,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -1263,10 +1260,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1283,10 +1280,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
         <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1303,10 +1300,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1323,7 +1320,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
@@ -1343,7 +1340,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
         <v>35</v>
@@ -1363,10 +1360,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
         <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>39</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -1376,6 +1373,26 @@
       </c>
       <c r="F17">
         <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1384,7 +1401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
updated num_lines based on TDP existing and planned lines
</commit_message>
<xml_diff>
--- a/data/num_lines.xlsx
+++ b/data/num_lines.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\pypsa-za\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\UbuntuPeter\home\joules\pypsa-za-v2\pypsa-za\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3029A53-E9CC-429D-8198-1F5404DC4800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435D82B1-7D07-4CB1-B96B-05C2AEB77BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RSA" sheetId="2" r:id="rId1"/>
@@ -631,8 +631,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1026,7 +1027,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1055,343 +1056,343 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
         <v>6</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>7</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>6</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <v>15</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D17" s="1">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>6</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="C18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17">
-        <v>3</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Messy draft - banking
</commit_message>
<xml_diff>
--- a/data/num_lines.xlsx
+++ b/data/num_lines.xlsx
@@ -5,24 +5,38 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\UbuntuPeter\home\joules\pypsa-za-v2\pypsa-za\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\pypsa-za\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435D82B1-7D07-4CB1-B96B-05C2AEB77BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5843FE9E-F782-489F-9D4E-BE0780078CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RSA" sheetId="2" r:id="rId1"/>
     <sheet name="9-supply" sheetId="3" r:id="rId2"/>
-    <sheet name="27-supply" sheetId="1" r:id="rId3"/>
+    <sheet name="10-supply" sheetId="4" r:id="rId3"/>
+    <sheet name="27-supply" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="44">
   <si>
     <t>name</t>
   </si>
@@ -148,6 +162,12 @@
   </si>
   <si>
     <t>KZN</t>
+  </si>
+  <si>
+    <t>NORTHERN CAPE 1</t>
+  </si>
+  <si>
+    <t>NORTHERN CAPE 2</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
@@ -1402,6 +1422,451 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF54E57-8F09-46B7-A762-D0AAF7E4520E}">
+  <dimension ref="A1:Q21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>7.1428571428571432</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>6.1278195488721723</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.2556390977443574</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.842105263157886</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4.5112781954887149</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>12.349624060150372</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.6729323308270572</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8.984962406015029</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>6.9924812030075145</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3.7593984962406002</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>7.1428571428571432</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2.6879699248120286</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>21.578947368421002</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>13.045112781954886</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>14.736842105263143</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>7.8571428571428577</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>15.601503759398431</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>3.0827067669172861</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1.842105263157886</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>

</xml_diff>